<commit_message>
bulk sql generator working
</commit_message>
<xml_diff>
--- a/datf_core/test/sqlbulk/bulk_sql_using_business_rules_1.xlsx
+++ b/datf_core/test/sqlbulk/bulk_sql_using_business_rules_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Workspaces\GitHub\DATF_Other\Pyspark\QE_ATF\datf_core\test\sqlbulk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6365A2-AF2C-4BFA-B1F9-9A673D3B13DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370EE4EA-5DD5-49E7-ADCD-12A70D9E7FEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,16 +49,16 @@
     <t>target</t>
   </si>
   <si>
-    <t>BIRTHPLACE, ADDRESS, CITY, STATE, COUNTY, ZIP, LAT, LON</t>
-  </si>
-  <si>
-    <t>this table consists of patient data admittied in clinics, using cte, create a qualified US postal address with these</t>
-  </si>
-  <si>
     <t>state_name, state_fips, state</t>
   </si>
   <si>
     <t>this table consist of medical diagnostic testing data, can you group by the columns and let me know which are the unique states participating</t>
+  </si>
+  <si>
+    <t>BIRTHPLACE, CITY</t>
+  </si>
+  <si>
+    <t>this table consists of patient data admittied in clinics, using cte, can you check which BIRTHPLACE are matching with CITY.</t>
   </si>
 </sst>
 </file>
@@ -436,7 +436,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="112.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,10 +477,10 @@
         <v>7</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -494,10 +494,10 @@
         <v>8</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>